<commit_message>
Actualizacion y borrado de checkpoints
</commit_message>
<xml_diff>
--- a/docs/Word_list2.xlsx
+++ b/docs/Word_list2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="284">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -494,6 +494,384 @@
   </si>
   <si>
     <t xml:space="preserve">punto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">earn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ganar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vacio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vaciar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enclose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">incluir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">encourage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">motor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fault</t>
+  </si>
+  <si>
+    <t xml:space="preserve">falta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">faulty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">con errores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">frame</t>
+  </si>
+  <si>
+    <t xml:space="preserve">marco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">congelar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proteger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suponer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guiar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hammer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">martillo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">martillar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">handle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harmful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">danino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harmless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inofensivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">altura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hesitate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dudar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">esconder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">impedir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">golpear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hollow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hueco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gancho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enganchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hurry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apuro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apurarse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hielo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">improve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mejorar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">improvement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mejora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inquire / enquire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">averiguar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inquiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">investigacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insurance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inward</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hacia adentro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saltar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">llave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nudo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lampara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sin grasa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pierna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prestar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">carga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cargar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cerradura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trancar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flojo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">holgado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loosen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aflojar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a alto volumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grumo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">masculino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">macho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gerenciar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gerencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fosforo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">combinar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">derretir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mistake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mezclar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mezcla</t>
   </si>
 </sst>
 </file>
@@ -508,6 +886,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -612,10 +991,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B116" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D132" activeCellId="0" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1757,7 +2136,875 @@
         <v>157</v>
       </c>
       <c r="D74" s="2"/>
-      <c r="E74" s="2" t="n">
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="n">
+        <v>171</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E75" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="n">
+        <v>172</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E76" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="E77" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="n">
+        <v>174</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="E78" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="E79" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="n">
+        <v>176</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="E80" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E81" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="n">
+        <v>178</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="E82" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="n">
+        <v>179</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E83" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="E84" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="n">
+        <v>181</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="E85" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="n">
+        <v>182</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E86" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="n">
+        <v>183</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="E87" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="n">
+        <v>184</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="D88" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="E88" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="D89" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="E89" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="n">
+        <v>186</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="D91" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="E91" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="E92" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="n">
+        <v>189</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="E93" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="E94" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="n">
+        <v>191</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="E95" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="n">
+        <v>192</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="E96" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="n">
+        <v>193</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E97" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="n">
+        <v>194</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E98" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="n">
+        <v>195</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="E99" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>211</v>
+      </c>
+      <c r="E100" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>213</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>214</v>
+      </c>
+      <c r="E101" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>216</v>
+      </c>
+      <c r="E102" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="n">
+        <v>199</v>
+      </c>
+      <c r="B103" s="0" t="s">
+        <v>217</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="E103" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="n">
+        <v>200</v>
+      </c>
+      <c r="B104" s="0" t="s">
+        <v>219</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>220</v>
+      </c>
+      <c r="E104" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="B105" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="E105" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="n">
+        <v>202</v>
+      </c>
+      <c r="B106" s="0" t="s">
+        <v>223</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="E106" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="n">
+        <v>203</v>
+      </c>
+      <c r="B107" s="0" t="s">
+        <v>225</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="E107" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="B108" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="E108" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="n">
+        <v>205</v>
+      </c>
+      <c r="B109" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>229</v>
+      </c>
+      <c r="E109" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="B110" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="C110" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="E110" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="n">
+        <v>207</v>
+      </c>
+      <c r="B111" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="C111" s="0" t="s">
+        <v>233</v>
+      </c>
+      <c r="D111" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="E111" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B112" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="C112" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="E112" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B113" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="C113" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="E113" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B114" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="C114" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="E114" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B115" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="C115" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="E115" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="B116" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="C116" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="E116" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="B117" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="C117" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="B118" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="E118" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="1" t="n">
+        <v>215</v>
+      </c>
+      <c r="B119" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="C119" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="D119" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="E119" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="B120" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="C120" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="D120" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="E120" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="B121" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="C121" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="E121" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="n">
+        <v>218</v>
+      </c>
+      <c r="B122" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="C122" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="B123" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="C123" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="E123" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="n">
+        <v>220</v>
+      </c>
+      <c r="B124" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="C124" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="D124" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="E124" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1" t="n">
+        <v>221</v>
+      </c>
+      <c r="B125" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="C125" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="E125" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="n">
+        <v>222</v>
+      </c>
+      <c r="B126" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="C126" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="E126" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="n">
+        <v>223</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C127" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="D127" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="E127" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="1" t="n">
+        <v>224</v>
+      </c>
+      <c r="B128" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="E128" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="1" t="n">
+        <v>225</v>
+      </c>
+      <c r="B129" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="E129" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="1" t="n">
+        <v>226</v>
+      </c>
+      <c r="B130" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D130" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="E130" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="1" t="n">
+        <v>227</v>
+      </c>
+      <c r="B131" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E131" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="1" t="n">
+        <v>228</v>
+      </c>
+      <c r="B132" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="C132" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="E132" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="B133" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C133" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="E133" s="2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>